<commit_message>
fix track to avoid cheating
</commit_message>
<xml_diff>
--- a/core/test/stf2.xlsx
+++ b/core/test/stf2.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\Environment-Framework\test\core_test\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\Environment-Framework\core\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AA64A95-914F-4E13-83EB-412CE2734253}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83634D52-0B9E-4E16-8A56-498B4BF1FD93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25180" windowHeight="16140" xr2:uid="{19C3DDC4-AFB1-4D82-AE89-12F56748A908}"/>
   </bookViews>
@@ -468,7 +468,7 @@
   <dimension ref="A1:AE21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AM25" sqref="AM25"/>
+      <selection activeCell="AM8" sqref="AM8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.26953125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -692,10 +692,10 @@
       <c r="K4" s="3"/>
       <c r="L4" s="3"/>
       <c r="M4" s="3"/>
-      <c r="N4" s="3"/>
-      <c r="O4" s="3"/>
-      <c r="P4" s="3"/>
-      <c r="Q4" s="3"/>
+      <c r="N4" s="2"/>
+      <c r="O4" s="2"/>
+      <c r="P4" s="2"/>
+      <c r="Q4" s="2"/>
       <c r="R4" s="3"/>
       <c r="S4" s="3"/>
       <c r="T4" s="3"/>
@@ -733,7 +733,7 @@
       <c r="N5" s="2"/>
       <c r="O5" s="2"/>
       <c r="P5" s="2"/>
-      <c r="Q5" s="3"/>
+      <c r="Q5" s="2"/>
       <c r="R5" s="3"/>
       <c r="S5" s="3"/>
       <c r="T5" s="3"/>
@@ -893,7 +893,7 @@
       <c r="N9" s="2"/>
       <c r="O9" s="2"/>
       <c r="P9" s="2"/>
-      <c r="Q9" s="3"/>
+      <c r="Q9" s="2"/>
       <c r="R9" s="3"/>
       <c r="S9" s="3"/>
       <c r="T9" s="3"/>
@@ -930,10 +930,10 @@
       <c r="K10" s="4"/>
       <c r="L10" s="4"/>
       <c r="M10" s="3"/>
-      <c r="N10" s="3"/>
-      <c r="O10" s="3"/>
-      <c r="P10" s="3"/>
-      <c r="Q10" s="3"/>
+      <c r="N10" s="2"/>
+      <c r="O10" s="2"/>
+      <c r="P10" s="2"/>
+      <c r="Q10" s="2"/>
       <c r="R10" s="3"/>
       <c r="S10" s="3"/>
       <c r="T10" s="3"/>

</xml_diff>

<commit_message>
deep q learning 3 option per dimension
</commit_message>
<xml_diff>
--- a/core/test/stf2.xlsx
+++ b/core/test/stf2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\Environment-Framework\core\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83634D52-0B9E-4E16-8A56-498B4BF1FD93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3A6D74F-F11E-44C3-BFAC-619799D8DBA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25180" windowHeight="16140" xr2:uid="{19C3DDC4-AFB1-4D82-AE89-12F56748A908}"/>
   </bookViews>
@@ -36,21 +36,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="2">
   <si>
     <t>&gt;</t>
   </si>
   <si>
-    <t>|</t>
-  </si>
-  <si>
-    <t>\</t>
-  </si>
-  <si>
     <t>/</t>
-  </si>
-  <si>
-    <t>&lt;</t>
   </si>
 </sst>
 </file>
@@ -66,7 +57,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -94,12 +85,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF0070C0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -131,7 +116,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -146,9 +131,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -468,7 +450,7 @@
   <dimension ref="A1:AE21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AM8" sqref="AM8"/>
+      <selection activeCell="O7" sqref="O7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.26953125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -725,7 +707,7 @@
       <c r="H5" s="3"/>
       <c r="I5" s="3"/>
       <c r="J5" s="3" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="K5" s="3"/>
       <c r="L5" s="3"/>
@@ -758,30 +740,72 @@
       <c r="C6" s="2"/>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="4"/>
-      <c r="I6" s="4"/>
-      <c r="J6" s="4" t="s">
+      <c r="F6" s="4">
+        <v>27</v>
+      </c>
+      <c r="G6" s="4">
+        <v>27</v>
+      </c>
+      <c r="H6" s="4">
+        <v>27</v>
+      </c>
+      <c r="I6" s="4">
+        <v>27</v>
+      </c>
+      <c r="J6" s="4">
+        <v>27</v>
+      </c>
+      <c r="K6" s="4">
+        <v>27</v>
+      </c>
+      <c r="L6" s="4">
+        <v>27</v>
+      </c>
+      <c r="M6" s="4">
+        <v>27</v>
+      </c>
+      <c r="N6" s="4">
+        <v>27</v>
+      </c>
+      <c r="O6" s="4">
+        <v>27</v>
+      </c>
+      <c r="P6" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="4">
+        <v>1</v>
+      </c>
+      <c r="R6" s="4">
+        <v>2</v>
+      </c>
+      <c r="S6" s="4">
         <v>3</v>
       </c>
-      <c r="K6" s="4"/>
-      <c r="L6" s="4"/>
-      <c r="M6" s="4"/>
-      <c r="N6" s="4"/>
-      <c r="O6" s="6"/>
-      <c r="P6" s="5"/>
-      <c r="Q6" s="4"/>
-      <c r="R6" s="4"/>
-      <c r="S6" s="4"/>
-      <c r="T6" s="4"/>
-      <c r="U6" s="4"/>
-      <c r="V6" s="4"/>
-      <c r="W6" s="4"/>
-      <c r="X6" s="4"/>
-      <c r="Y6" s="4"/>
-      <c r="Z6" s="4"/>
-      <c r="AA6" s="4"/>
+      <c r="T6" s="4">
+        <v>4</v>
+      </c>
+      <c r="U6" s="4">
+        <v>5</v>
+      </c>
+      <c r="V6" s="4">
+        <v>6</v>
+      </c>
+      <c r="W6" s="4">
+        <v>7</v>
+      </c>
+      <c r="X6" s="4">
+        <v>8</v>
+      </c>
+      <c r="Y6" s="4">
+        <v>9</v>
+      </c>
+      <c r="Z6" s="4">
+        <v>10</v>
+      </c>
+      <c r="AA6" s="4">
+        <v>11</v>
+      </c>
       <c r="AB6" s="3"/>
       <c r="AC6" s="3"/>
       <c r="AD6" s="2"/>
@@ -796,36 +820,72 @@
       <c r="C7" s="2"/>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
-      <c r="H7" s="4"/>
-      <c r="I7" s="4" t="s">
+      <c r="F7" s="4">
+        <v>26</v>
+      </c>
+      <c r="G7" s="4">
+        <v>26</v>
+      </c>
+      <c r="H7" s="4">
+        <v>26</v>
+      </c>
+      <c r="I7" s="4">
+        <v>26</v>
+      </c>
+      <c r="J7" s="4">
+        <v>26</v>
+      </c>
+      <c r="K7" s="4">
+        <v>26</v>
+      </c>
+      <c r="L7" s="4">
+        <v>26</v>
+      </c>
+      <c r="M7" s="4">
+        <v>26</v>
+      </c>
+      <c r="N7" s="4">
+        <v>26</v>
+      </c>
+      <c r="O7" s="4">
+        <v>27</v>
+      </c>
+      <c r="P7" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="4">
+        <v>1</v>
+      </c>
+      <c r="R7" s="4">
+        <v>2</v>
+      </c>
+      <c r="S7" s="4">
         <v>3</v>
       </c>
-      <c r="J7" s="4"/>
-      <c r="K7" s="4"/>
-      <c r="L7" s="4"/>
-      <c r="M7" s="4"/>
-      <c r="N7" s="4"/>
-      <c r="O7" s="6"/>
-      <c r="P7" s="5"/>
-      <c r="Q7" s="4"/>
-      <c r="R7" s="4"/>
-      <c r="S7" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="T7" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="U7" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="V7" s="4"/>
-      <c r="W7" s="4"/>
-      <c r="X7" s="4"/>
-      <c r="Y7" s="4"/>
-      <c r="Z7" s="4"/>
-      <c r="AA7" s="4"/>
+      <c r="T7" s="4">
+        <v>4</v>
+      </c>
+      <c r="U7" s="4">
+        <v>5</v>
+      </c>
+      <c r="V7" s="4">
+        <v>6</v>
+      </c>
+      <c r="W7" s="4">
+        <v>7</v>
+      </c>
+      <c r="X7" s="4">
+        <v>8</v>
+      </c>
+      <c r="Y7" s="4">
+        <v>9</v>
+      </c>
+      <c r="Z7" s="4">
+        <v>10</v>
+      </c>
+      <c r="AA7" s="4">
+        <v>11</v>
+      </c>
       <c r="AB7" s="3"/>
       <c r="AC7" s="3"/>
       <c r="AD7" s="2"/>
@@ -840,32 +900,72 @@
       <c r="C8" s="2"/>
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
-      <c r="H8" s="4"/>
-      <c r="I8" s="4" t="s">
+      <c r="F8" s="4">
+        <v>25</v>
+      </c>
+      <c r="G8" s="4">
+        <v>25</v>
+      </c>
+      <c r="H8" s="4">
+        <v>25</v>
+      </c>
+      <c r="I8" s="4">
+        <v>25</v>
+      </c>
+      <c r="J8" s="4">
+        <v>25</v>
+      </c>
+      <c r="K8" s="4">
+        <v>25</v>
+      </c>
+      <c r="L8" s="4">
+        <v>25</v>
+      </c>
+      <c r="M8" s="4">
+        <v>25</v>
+      </c>
+      <c r="N8" s="4">
+        <v>26</v>
+      </c>
+      <c r="O8" s="4">
+        <v>27</v>
+      </c>
+      <c r="P8" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q8" s="4">
         <v>1</v>
       </c>
-      <c r="J8" s="4"/>
-      <c r="K8" s="4"/>
-      <c r="L8" s="4"/>
-      <c r="M8" s="4"/>
-      <c r="N8" s="4"/>
-      <c r="O8" s="6"/>
-      <c r="P8" s="5"/>
-      <c r="Q8" s="4"/>
-      <c r="R8" s="4"/>
-      <c r="S8" s="4"/>
-      <c r="T8" s="4"/>
-      <c r="U8" s="4" t="s">
+      <c r="R8" s="4">
         <v>2</v>
       </c>
-      <c r="V8" s="4"/>
-      <c r="W8" s="4"/>
-      <c r="X8" s="4"/>
-      <c r="Y8" s="4"/>
-      <c r="Z8" s="4"/>
-      <c r="AA8" s="4"/>
+      <c r="S8" s="4">
+        <v>3</v>
+      </c>
+      <c r="T8" s="4">
+        <v>4</v>
+      </c>
+      <c r="U8" s="4">
+        <v>5</v>
+      </c>
+      <c r="V8" s="4">
+        <v>6</v>
+      </c>
+      <c r="W8" s="4">
+        <v>7</v>
+      </c>
+      <c r="X8" s="4">
+        <v>8</v>
+      </c>
+      <c r="Y8" s="4">
+        <v>9</v>
+      </c>
+      <c r="Z8" s="4">
+        <v>10</v>
+      </c>
+      <c r="AA8" s="4">
+        <v>11</v>
+      </c>
       <c r="AB8" s="3"/>
       <c r="AC8" s="3"/>
       <c r="AD8" s="2"/>
@@ -880,15 +980,27 @@
       <c r="C9" s="2"/>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
-      <c r="H9" s="4"/>
-      <c r="I9" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="J9" s="4"/>
-      <c r="K9" s="4"/>
-      <c r="L9" s="4"/>
+      <c r="F9" s="4">
+        <v>25</v>
+      </c>
+      <c r="G9" s="4">
+        <v>24</v>
+      </c>
+      <c r="H9" s="4">
+        <v>24</v>
+      </c>
+      <c r="I9" s="4">
+        <v>24</v>
+      </c>
+      <c r="J9" s="4">
+        <v>24</v>
+      </c>
+      <c r="K9" s="4">
+        <v>24</v>
+      </c>
+      <c r="L9" s="4">
+        <v>24</v>
+      </c>
       <c r="M9" s="3"/>
       <c r="N9" s="2"/>
       <c r="O9" s="2"/>
@@ -897,15 +1009,27 @@
       <c r="R9" s="3"/>
       <c r="S9" s="3"/>
       <c r="T9" s="3"/>
-      <c r="U9" s="4"/>
-      <c r="V9" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="W9" s="4"/>
-      <c r="X9" s="4"/>
-      <c r="Y9" s="4"/>
-      <c r="Z9" s="4"/>
-      <c r="AA9" s="4"/>
+      <c r="U9" s="4">
+        <v>5</v>
+      </c>
+      <c r="V9" s="4">
+        <v>6</v>
+      </c>
+      <c r="W9" s="4">
+        <v>7</v>
+      </c>
+      <c r="X9" s="4">
+        <v>8</v>
+      </c>
+      <c r="Y9" s="4">
+        <v>9</v>
+      </c>
+      <c r="Z9" s="4">
+        <v>10</v>
+      </c>
+      <c r="AA9" s="4">
+        <v>11</v>
+      </c>
       <c r="AB9" s="3"/>
       <c r="AC9" s="3"/>
       <c r="AD9" s="2"/>
@@ -920,15 +1044,27 @@
       <c r="C10" s="2"/>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
-      <c r="H10" s="4"/>
-      <c r="I10" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="J10" s="4"/>
-      <c r="K10" s="4"/>
-      <c r="L10" s="4"/>
+      <c r="F10" s="4">
+        <v>25</v>
+      </c>
+      <c r="G10" s="4">
+        <v>24</v>
+      </c>
+      <c r="H10" s="4">
+        <v>23</v>
+      </c>
+      <c r="I10" s="4">
+        <v>23</v>
+      </c>
+      <c r="J10" s="4">
+        <v>23</v>
+      </c>
+      <c r="K10" s="4">
+        <v>23</v>
+      </c>
+      <c r="L10" s="4">
+        <v>23</v>
+      </c>
       <c r="M10" s="3"/>
       <c r="N10" s="2"/>
       <c r="O10" s="2"/>
@@ -937,15 +1073,27 @@
       <c r="R10" s="3"/>
       <c r="S10" s="3"/>
       <c r="T10" s="3"/>
-      <c r="U10" s="4"/>
-      <c r="V10" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="W10" s="4"/>
-      <c r="X10" s="4"/>
-      <c r="Y10" s="4"/>
-      <c r="Z10" s="4"/>
-      <c r="AA10" s="4"/>
+      <c r="U10" s="4">
+        <v>6</v>
+      </c>
+      <c r="V10" s="4">
+        <v>6</v>
+      </c>
+      <c r="W10" s="4">
+        <v>7</v>
+      </c>
+      <c r="X10" s="4">
+        <v>8</v>
+      </c>
+      <c r="Y10" s="4">
+        <v>9</v>
+      </c>
+      <c r="Z10" s="4">
+        <v>10</v>
+      </c>
+      <c r="AA10" s="4">
+        <v>11</v>
+      </c>
       <c r="AB10" s="3"/>
       <c r="AC10" s="3"/>
       <c r="AD10" s="2"/>
@@ -960,15 +1108,27 @@
       <c r="C11" s="2"/>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
-      <c r="H11" s="4"/>
-      <c r="I11" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="J11" s="4"/>
-      <c r="K11" s="4"/>
-      <c r="L11" s="4"/>
+      <c r="F11" s="4">
+        <v>25</v>
+      </c>
+      <c r="G11" s="4">
+        <v>24</v>
+      </c>
+      <c r="H11" s="4">
+        <v>23</v>
+      </c>
+      <c r="I11" s="4">
+        <v>22</v>
+      </c>
+      <c r="J11" s="4">
+        <v>22</v>
+      </c>
+      <c r="K11" s="4">
+        <v>22</v>
+      </c>
+      <c r="L11" s="4">
+        <v>22</v>
+      </c>
       <c r="M11" s="3"/>
       <c r="N11" s="3"/>
       <c r="O11" s="2"/>
@@ -977,15 +1137,27 @@
       <c r="R11" s="2"/>
       <c r="S11" s="3"/>
       <c r="T11" s="3"/>
-      <c r="U11" s="4"/>
-      <c r="V11" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="W11" s="4"/>
-      <c r="X11" s="4"/>
-      <c r="Y11" s="4"/>
-      <c r="Z11" s="4"/>
-      <c r="AA11" s="4"/>
+      <c r="U11" s="4">
+        <v>7</v>
+      </c>
+      <c r="V11" s="4">
+        <v>7</v>
+      </c>
+      <c r="W11" s="4">
+        <v>7</v>
+      </c>
+      <c r="X11" s="4">
+        <v>8</v>
+      </c>
+      <c r="Y11" s="4">
+        <v>9</v>
+      </c>
+      <c r="Z11" s="4">
+        <v>10</v>
+      </c>
+      <c r="AA11" s="4">
+        <v>11</v>
+      </c>
       <c r="AB11" s="3"/>
       <c r="AC11" s="3"/>
       <c r="AD11" s="2"/>
@@ -1000,15 +1172,27 @@
       <c r="C12" s="2"/>
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
-      <c r="F12" s="4"/>
-      <c r="G12" s="4"/>
-      <c r="H12" s="4"/>
-      <c r="I12" s="4"/>
-      <c r="J12" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="K12" s="4"/>
-      <c r="L12" s="4"/>
+      <c r="F12" s="4">
+        <v>25</v>
+      </c>
+      <c r="G12" s="4">
+        <v>24</v>
+      </c>
+      <c r="H12" s="4">
+        <v>23</v>
+      </c>
+      <c r="I12" s="4">
+        <v>22</v>
+      </c>
+      <c r="J12" s="4">
+        <v>21</v>
+      </c>
+      <c r="K12" s="4">
+        <v>21</v>
+      </c>
+      <c r="L12" s="4">
+        <v>21</v>
+      </c>
       <c r="M12" s="3"/>
       <c r="N12" s="3"/>
       <c r="O12" s="2"/>
@@ -1017,15 +1201,27 @@
       <c r="R12" s="2"/>
       <c r="S12" s="3"/>
       <c r="T12" s="3"/>
-      <c r="U12" s="4"/>
-      <c r="V12" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="W12" s="4"/>
-      <c r="X12" s="4"/>
-      <c r="Y12" s="4"/>
-      <c r="Z12" s="4"/>
-      <c r="AA12" s="4"/>
+      <c r="U12" s="4">
+        <v>8</v>
+      </c>
+      <c r="V12" s="4">
+        <v>8</v>
+      </c>
+      <c r="W12" s="4">
+        <v>8</v>
+      </c>
+      <c r="X12" s="4">
+        <v>8</v>
+      </c>
+      <c r="Y12" s="4">
+        <v>9</v>
+      </c>
+      <c r="Z12" s="4">
+        <v>10</v>
+      </c>
+      <c r="AA12" s="4">
+        <v>11</v>
+      </c>
       <c r="AB12" s="3"/>
       <c r="AC12" s="3"/>
       <c r="AD12" s="2"/>
@@ -1040,15 +1236,27 @@
       <c r="C13" s="2"/>
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
-      <c r="F13" s="4"/>
-      <c r="G13" s="4"/>
-      <c r="H13" s="4"/>
-      <c r="I13" s="4"/>
-      <c r="J13" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="K13" s="4"/>
-      <c r="L13" s="4"/>
+      <c r="F13" s="4">
+        <v>25</v>
+      </c>
+      <c r="G13" s="4">
+        <v>24</v>
+      </c>
+      <c r="H13" s="4">
+        <v>23</v>
+      </c>
+      <c r="I13" s="4">
+        <v>22</v>
+      </c>
+      <c r="J13" s="4">
+        <v>21</v>
+      </c>
+      <c r="K13" s="4">
+        <v>20</v>
+      </c>
+      <c r="L13" s="4">
+        <v>20</v>
+      </c>
       <c r="M13" s="3"/>
       <c r="N13" s="3"/>
       <c r="O13" s="3"/>
@@ -1057,15 +1265,27 @@
       <c r="R13" s="3"/>
       <c r="S13" s="3"/>
       <c r="T13" s="3"/>
-      <c r="U13" s="4"/>
-      <c r="V13" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="W13" s="4"/>
-      <c r="X13" s="4"/>
-      <c r="Y13" s="4"/>
-      <c r="Z13" s="4"/>
-      <c r="AA13" s="4"/>
+      <c r="U13" s="4">
+        <v>9</v>
+      </c>
+      <c r="V13" s="4">
+        <v>9</v>
+      </c>
+      <c r="W13" s="4">
+        <v>9</v>
+      </c>
+      <c r="X13" s="4">
+        <v>9</v>
+      </c>
+      <c r="Y13" s="4">
+        <v>9</v>
+      </c>
+      <c r="Z13" s="4">
+        <v>10</v>
+      </c>
+      <c r="AA13" s="4">
+        <v>11</v>
+      </c>
       <c r="AB13" s="3"/>
       <c r="AC13" s="3"/>
       <c r="AD13" s="2"/>
@@ -1080,15 +1300,27 @@
       <c r="C14" s="2"/>
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
-      <c r="F14" s="4"/>
-      <c r="G14" s="4"/>
-      <c r="H14" s="4"/>
-      <c r="I14" s="4"/>
-      <c r="J14" s="4"/>
-      <c r="K14" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="L14" s="4"/>
+      <c r="F14" s="4">
+        <v>25</v>
+      </c>
+      <c r="G14" s="4">
+        <v>24</v>
+      </c>
+      <c r="H14" s="4">
+        <v>23</v>
+      </c>
+      <c r="I14" s="4">
+        <v>22</v>
+      </c>
+      <c r="J14" s="4">
+        <v>21</v>
+      </c>
+      <c r="K14" s="4">
+        <v>20</v>
+      </c>
+      <c r="L14" s="4">
+        <v>19</v>
+      </c>
       <c r="M14" s="3"/>
       <c r="N14" s="3"/>
       <c r="O14" s="3"/>
@@ -1097,17 +1329,27 @@
       <c r="R14" s="3"/>
       <c r="S14" s="3"/>
       <c r="T14" s="3"/>
-      <c r="U14" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="V14" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="W14" s="4"/>
-      <c r="X14" s="4"/>
-      <c r="Y14" s="4"/>
-      <c r="Z14" s="4"/>
-      <c r="AA14" s="4"/>
+      <c r="U14" s="4">
+        <v>10</v>
+      </c>
+      <c r="V14" s="4">
+        <v>10</v>
+      </c>
+      <c r="W14" s="4">
+        <v>10</v>
+      </c>
+      <c r="X14" s="4">
+        <v>10</v>
+      </c>
+      <c r="Y14" s="4">
+        <v>10</v>
+      </c>
+      <c r="Z14" s="4">
+        <v>10</v>
+      </c>
+      <c r="AA14" s="4">
+        <v>11</v>
+      </c>
       <c r="AB14" s="3"/>
       <c r="AC14" s="3"/>
       <c r="AD14" s="2"/>
@@ -1122,34 +1364,72 @@
       <c r="C15" s="2"/>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
-      <c r="F15" s="4"/>
-      <c r="G15" s="4"/>
-      <c r="H15" s="4"/>
-      <c r="I15" s="4"/>
-      <c r="J15" s="4"/>
-      <c r="K15" s="4"/>
-      <c r="L15" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="M15" s="4"/>
-      <c r="N15" s="4"/>
-      <c r="O15" s="4"/>
-      <c r="P15" s="4"/>
-      <c r="Q15" s="4"/>
-      <c r="R15" s="4"/>
-      <c r="S15" s="4"/>
-      <c r="T15" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="U15" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="V15" s="4"/>
-      <c r="W15" s="4"/>
-      <c r="X15" s="4"/>
-      <c r="Y15" s="4"/>
-      <c r="Z15" s="4"/>
-      <c r="AA15" s="4"/>
+      <c r="F15" s="4">
+        <v>25</v>
+      </c>
+      <c r="G15" s="4">
+        <v>24</v>
+      </c>
+      <c r="H15" s="4">
+        <v>23</v>
+      </c>
+      <c r="I15" s="4">
+        <v>22</v>
+      </c>
+      <c r="J15" s="4">
+        <v>21</v>
+      </c>
+      <c r="K15" s="4">
+        <v>20</v>
+      </c>
+      <c r="L15" s="4">
+        <v>19</v>
+      </c>
+      <c r="M15" s="4">
+        <v>18</v>
+      </c>
+      <c r="N15" s="4">
+        <v>17</v>
+      </c>
+      <c r="O15" s="4">
+        <v>16</v>
+      </c>
+      <c r="P15" s="4">
+        <v>15</v>
+      </c>
+      <c r="Q15" s="4">
+        <v>14</v>
+      </c>
+      <c r="R15" s="4">
+        <v>13</v>
+      </c>
+      <c r="S15" s="4">
+        <v>12</v>
+      </c>
+      <c r="T15" s="4">
+        <v>11</v>
+      </c>
+      <c r="U15" s="4">
+        <v>11</v>
+      </c>
+      <c r="V15" s="4">
+        <v>11</v>
+      </c>
+      <c r="W15" s="4">
+        <v>11</v>
+      </c>
+      <c r="X15" s="4">
+        <v>11</v>
+      </c>
+      <c r="Y15" s="4">
+        <v>11</v>
+      </c>
+      <c r="Z15" s="4">
+        <v>11</v>
+      </c>
+      <c r="AA15" s="4">
+        <v>11</v>
+      </c>
       <c r="AB15" s="3"/>
       <c r="AC15" s="3"/>
       <c r="AD15" s="2"/>
@@ -1164,42 +1444,72 @@
       <c r="C16" s="2"/>
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
-      <c r="F16" s="4"/>
-      <c r="G16" s="4"/>
-      <c r="H16" s="4"/>
-      <c r="I16" s="4"/>
-      <c r="J16" s="4"/>
-      <c r="K16" s="4"/>
-      <c r="L16" s="4"/>
-      <c r="M16" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="N16" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="O16" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="P16" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q16" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="R16" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="S16" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="T16" s="4"/>
-      <c r="U16" s="4"/>
-      <c r="V16" s="4"/>
-      <c r="W16" s="4"/>
-      <c r="X16" s="4"/>
-      <c r="Y16" s="4"/>
-      <c r="Z16" s="4"/>
-      <c r="AA16" s="4"/>
+      <c r="F16" s="4">
+        <v>25</v>
+      </c>
+      <c r="G16" s="4">
+        <v>24</v>
+      </c>
+      <c r="H16" s="4">
+        <v>23</v>
+      </c>
+      <c r="I16" s="4">
+        <v>22</v>
+      </c>
+      <c r="J16" s="4">
+        <v>21</v>
+      </c>
+      <c r="K16" s="4">
+        <v>20</v>
+      </c>
+      <c r="L16" s="4">
+        <v>19</v>
+      </c>
+      <c r="M16" s="4">
+        <v>18</v>
+      </c>
+      <c r="N16" s="4">
+        <v>17</v>
+      </c>
+      <c r="O16" s="4">
+        <v>16</v>
+      </c>
+      <c r="P16" s="4">
+        <v>15</v>
+      </c>
+      <c r="Q16" s="4">
+        <v>14</v>
+      </c>
+      <c r="R16" s="4">
+        <v>13</v>
+      </c>
+      <c r="S16" s="4">
+        <v>12</v>
+      </c>
+      <c r="T16" s="4">
+        <v>12</v>
+      </c>
+      <c r="U16" s="4">
+        <v>12</v>
+      </c>
+      <c r="V16" s="4">
+        <v>12</v>
+      </c>
+      <c r="W16" s="4">
+        <v>12</v>
+      </c>
+      <c r="X16" s="4">
+        <v>12</v>
+      </c>
+      <c r="Y16" s="4">
+        <v>12</v>
+      </c>
+      <c r="Z16" s="4">
+        <v>12</v>
+      </c>
+      <c r="AA16" s="4">
+        <v>12</v>
+      </c>
       <c r="AB16" s="3"/>
       <c r="AC16" s="3"/>
       <c r="AD16" s="2"/>
@@ -1214,28 +1524,72 @@
       <c r="C17" s="2"/>
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>
-      <c r="F17" s="4"/>
-      <c r="G17" s="4"/>
-      <c r="H17" s="4"/>
-      <c r="I17" s="4"/>
-      <c r="J17" s="4"/>
-      <c r="K17" s="4"/>
-      <c r="L17" s="4"/>
-      <c r="M17" s="4"/>
-      <c r="N17" s="4"/>
-      <c r="O17" s="4"/>
-      <c r="P17" s="4"/>
-      <c r="Q17" s="4"/>
-      <c r="R17" s="4"/>
-      <c r="S17" s="4"/>
-      <c r="T17" s="4"/>
-      <c r="U17" s="4"/>
-      <c r="V17" s="4"/>
-      <c r="W17" s="4"/>
-      <c r="X17" s="4"/>
-      <c r="Y17" s="4"/>
-      <c r="Z17" s="4"/>
-      <c r="AA17" s="4"/>
+      <c r="F17" s="4">
+        <v>25</v>
+      </c>
+      <c r="G17" s="4">
+        <v>24</v>
+      </c>
+      <c r="H17" s="4">
+        <v>23</v>
+      </c>
+      <c r="I17" s="4">
+        <v>22</v>
+      </c>
+      <c r="J17" s="4">
+        <v>21</v>
+      </c>
+      <c r="K17" s="4">
+        <v>20</v>
+      </c>
+      <c r="L17" s="4">
+        <v>19</v>
+      </c>
+      <c r="M17" s="4">
+        <v>18</v>
+      </c>
+      <c r="N17" s="4">
+        <v>17</v>
+      </c>
+      <c r="O17" s="4">
+        <v>16</v>
+      </c>
+      <c r="P17" s="4">
+        <v>15</v>
+      </c>
+      <c r="Q17" s="4">
+        <v>14</v>
+      </c>
+      <c r="R17" s="4">
+        <v>13</v>
+      </c>
+      <c r="S17" s="4">
+        <v>13</v>
+      </c>
+      <c r="T17" s="4">
+        <v>13</v>
+      </c>
+      <c r="U17" s="4">
+        <v>13</v>
+      </c>
+      <c r="V17" s="4">
+        <v>13</v>
+      </c>
+      <c r="W17" s="4">
+        <v>13</v>
+      </c>
+      <c r="X17" s="4">
+        <v>13</v>
+      </c>
+      <c r="Y17" s="4">
+        <v>13</v>
+      </c>
+      <c r="Z17" s="4">
+        <v>13</v>
+      </c>
+      <c r="AA17" s="4">
+        <v>13</v>
+      </c>
       <c r="AB17" s="3"/>
       <c r="AC17" s="3"/>
       <c r="AD17" s="2"/>

</xml_diff>

<commit_message>
Add reverse pass in track distance calculation
</commit_message>
<xml_diff>
--- a/core/test/stf2.xlsx
+++ b/core/test/stf2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\Environment-Framework\core\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3A6D74F-F11E-44C3-BFAC-619799D8DBA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9083F94-B052-40BE-86B8-8F927CF63590}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25180" windowHeight="16140" xr2:uid="{19C3DDC4-AFB1-4D82-AE89-12F56748A908}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="2">
   <si>
     <t>&gt;</t>
   </si>
@@ -447,10 +447,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FBDCF30-EC86-426C-99D7-AF955C90BE99}">
-  <dimension ref="A1:AE21"/>
+  <dimension ref="A1:AE45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O7" sqref="O7"/>
+      <selection activeCell="AQ20" sqref="AQ20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.26953125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1739,6 +1739,1287 @@
       <c r="AD21" s="2"/>
       <c r="AE21" s="2"/>
     </row>
+    <row r="25" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A25" s="1">
+        <v>0</v>
+      </c>
+      <c r="B25" s="1">
+        <v>0</v>
+      </c>
+      <c r="C25" s="1">
+        <f t="shared" ref="C25" si="2">B25+1</f>
+        <v>1</v>
+      </c>
+      <c r="D25" s="1">
+        <f t="shared" ref="D25" si="3">C25+1</f>
+        <v>2</v>
+      </c>
+      <c r="E25" s="1">
+        <f t="shared" ref="E25" si="4">D25+1</f>
+        <v>3</v>
+      </c>
+      <c r="F25" s="1">
+        <f t="shared" ref="F25" si="5">E25+1</f>
+        <v>4</v>
+      </c>
+      <c r="G25" s="1">
+        <f t="shared" ref="G25" si="6">F25+1</f>
+        <v>5</v>
+      </c>
+      <c r="H25" s="1">
+        <f t="shared" ref="H25" si="7">G25+1</f>
+        <v>6</v>
+      </c>
+      <c r="I25" s="1">
+        <f t="shared" ref="I25" si="8">H25+1</f>
+        <v>7</v>
+      </c>
+      <c r="J25" s="1">
+        <f t="shared" ref="J25" si="9">I25+1</f>
+        <v>8</v>
+      </c>
+      <c r="K25" s="1">
+        <f t="shared" ref="K25" si="10">J25+1</f>
+        <v>9</v>
+      </c>
+      <c r="L25" s="1">
+        <f t="shared" ref="L25" si="11">K25+1</f>
+        <v>10</v>
+      </c>
+      <c r="M25" s="1">
+        <f t="shared" ref="M25" si="12">L25+1</f>
+        <v>11</v>
+      </c>
+      <c r="N25" s="1">
+        <f t="shared" ref="N25" si="13">M25+1</f>
+        <v>12</v>
+      </c>
+      <c r="O25" s="1">
+        <f t="shared" ref="O25" si="14">N25+1</f>
+        <v>13</v>
+      </c>
+      <c r="P25" s="1">
+        <f t="shared" ref="P25" si="15">O25+1</f>
+        <v>14</v>
+      </c>
+      <c r="Q25" s="1">
+        <f t="shared" ref="Q25" si="16">P25+1</f>
+        <v>15</v>
+      </c>
+      <c r="R25" s="1">
+        <f t="shared" ref="R25" si="17">Q25+1</f>
+        <v>16</v>
+      </c>
+      <c r="S25" s="1">
+        <f t="shared" ref="S25" si="18">R25+1</f>
+        <v>17</v>
+      </c>
+      <c r="T25" s="1">
+        <f t="shared" ref="T25" si="19">S25+1</f>
+        <v>18</v>
+      </c>
+      <c r="U25" s="1">
+        <f t="shared" ref="U25" si="20">T25+1</f>
+        <v>19</v>
+      </c>
+      <c r="V25" s="1">
+        <f t="shared" ref="V25" si="21">U25+1</f>
+        <v>20</v>
+      </c>
+      <c r="W25" s="1">
+        <f t="shared" ref="W25" si="22">V25+1</f>
+        <v>21</v>
+      </c>
+      <c r="X25" s="1">
+        <f t="shared" ref="X25" si="23">W25+1</f>
+        <v>22</v>
+      </c>
+      <c r="Y25" s="1">
+        <f t="shared" ref="Y25" si="24">X25+1</f>
+        <v>23</v>
+      </c>
+      <c r="Z25" s="1">
+        <f t="shared" ref="Z25" si="25">Y25+1</f>
+        <v>24</v>
+      </c>
+      <c r="AA25" s="1">
+        <f t="shared" ref="AA25" si="26">Z25+1</f>
+        <v>25</v>
+      </c>
+      <c r="AB25" s="1">
+        <f t="shared" ref="AB25" si="27">AA25+1</f>
+        <v>26</v>
+      </c>
+      <c r="AC25" s="1">
+        <f t="shared" ref="AC25" si="28">AB25+1</f>
+        <v>27</v>
+      </c>
+      <c r="AD25" s="1">
+        <f t="shared" ref="AD25" si="29">AC25+1</f>
+        <v>28</v>
+      </c>
+      <c r="AE25" s="1">
+        <f t="shared" ref="AE25" si="30">AD25+1</f>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="26" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A26" s="1">
+        <v>0</v>
+      </c>
+      <c r="B26" s="2"/>
+      <c r="C26" s="2"/>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
+      <c r="F26" s="2"/>
+      <c r="G26" s="2"/>
+      <c r="H26" s="2"/>
+      <c r="I26" s="2"/>
+      <c r="J26" s="2"/>
+      <c r="K26" s="2"/>
+      <c r="L26" s="2"/>
+      <c r="M26" s="2"/>
+      <c r="N26" s="2"/>
+      <c r="O26" s="2"/>
+      <c r="P26" s="2"/>
+      <c r="Q26" s="2"/>
+      <c r="R26" s="2"/>
+      <c r="S26" s="2"/>
+      <c r="T26" s="2"/>
+      <c r="U26" s="2"/>
+      <c r="V26" s="2"/>
+      <c r="W26" s="2"/>
+      <c r="X26" s="2"/>
+      <c r="Y26" s="2"/>
+      <c r="Z26" s="2"/>
+      <c r="AA26" s="2"/>
+      <c r="AB26" s="2"/>
+      <c r="AC26" s="2"/>
+      <c r="AD26" s="2"/>
+      <c r="AE26" s="2"/>
+    </row>
+    <row r="27" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A27" s="1">
+        <f t="shared" ref="A27:A45" si="31">A26+1</f>
+        <v>1</v>
+      </c>
+      <c r="B27" s="2"/>
+      <c r="C27" s="2"/>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2"/>
+      <c r="F27" s="2"/>
+      <c r="G27" s="2"/>
+      <c r="H27" s="2"/>
+      <c r="I27" s="2"/>
+      <c r="J27" s="2"/>
+      <c r="K27" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="L27" s="2"/>
+      <c r="M27" s="2"/>
+      <c r="N27" s="2"/>
+      <c r="O27" s="2"/>
+      <c r="P27" s="2"/>
+      <c r="Q27" s="2"/>
+      <c r="R27" s="2"/>
+      <c r="S27" s="2"/>
+      <c r="T27" s="2"/>
+      <c r="U27" s="2"/>
+      <c r="V27" s="2"/>
+      <c r="W27" s="2"/>
+      <c r="X27" s="2"/>
+      <c r="Y27" s="2"/>
+      <c r="Z27" s="2"/>
+      <c r="AA27" s="2"/>
+      <c r="AB27" s="2"/>
+      <c r="AC27" s="2"/>
+      <c r="AD27" s="2"/>
+      <c r="AE27" s="2"/>
+    </row>
+    <row r="28" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A28" s="1">
+        <f t="shared" si="31"/>
+        <v>2</v>
+      </c>
+      <c r="B28" s="2"/>
+      <c r="C28" s="2"/>
+      <c r="D28" s="3"/>
+      <c r="E28" s="3"/>
+      <c r="F28" s="3"/>
+      <c r="G28" s="3"/>
+      <c r="H28" s="3"/>
+      <c r="I28" s="3"/>
+      <c r="J28" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="K28" s="3"/>
+      <c r="L28" s="3"/>
+      <c r="M28" s="3"/>
+      <c r="N28" s="2"/>
+      <c r="O28" s="2"/>
+      <c r="P28" s="2"/>
+      <c r="Q28" s="2"/>
+      <c r="R28" s="3"/>
+      <c r="S28" s="3"/>
+      <c r="T28" s="3"/>
+      <c r="U28" s="3"/>
+      <c r="V28" s="3"/>
+      <c r="W28" s="3"/>
+      <c r="X28" s="3"/>
+      <c r="Y28" s="3"/>
+      <c r="Z28" s="3"/>
+      <c r="AA28" s="3"/>
+      <c r="AB28" s="3"/>
+      <c r="AC28" s="3"/>
+      <c r="AD28" s="2"/>
+      <c r="AE28" s="2"/>
+    </row>
+    <row r="29" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A29" s="1">
+        <f t="shared" si="31"/>
+        <v>3</v>
+      </c>
+      <c r="B29" s="2"/>
+      <c r="C29" s="2"/>
+      <c r="D29" s="3"/>
+      <c r="E29" s="3"/>
+      <c r="F29" s="3"/>
+      <c r="G29" s="3"/>
+      <c r="H29" s="3"/>
+      <c r="I29" s="3"/>
+      <c r="J29" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="K29" s="3"/>
+      <c r="L29" s="3"/>
+      <c r="M29" s="3"/>
+      <c r="N29" s="2"/>
+      <c r="O29" s="2"/>
+      <c r="P29" s="2"/>
+      <c r="Q29" s="2"/>
+      <c r="R29" s="3"/>
+      <c r="S29" s="3"/>
+      <c r="T29" s="3"/>
+      <c r="U29" s="3"/>
+      <c r="V29" s="3"/>
+      <c r="W29" s="3"/>
+      <c r="X29" s="3"/>
+      <c r="Y29" s="3"/>
+      <c r="Z29" s="3"/>
+      <c r="AA29" s="3"/>
+      <c r="AB29" s="3"/>
+      <c r="AC29" s="3"/>
+      <c r="AD29" s="2"/>
+      <c r="AE29" s="2"/>
+    </row>
+    <row r="30" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A30" s="1">
+        <f t="shared" si="31"/>
+        <v>4</v>
+      </c>
+      <c r="B30" s="2"/>
+      <c r="C30" s="2"/>
+      <c r="D30" s="3"/>
+      <c r="E30" s="3"/>
+      <c r="F30" s="4">
+        <v>18</v>
+      </c>
+      <c r="G30" s="4">
+        <v>19</v>
+      </c>
+      <c r="H30" s="4">
+        <v>20</v>
+      </c>
+      <c r="I30" s="4">
+        <v>21</v>
+      </c>
+      <c r="J30" s="4">
+        <v>22</v>
+      </c>
+      <c r="K30" s="4">
+        <v>23</v>
+      </c>
+      <c r="L30" s="4">
+        <v>24</v>
+      </c>
+      <c r="M30" s="4">
+        <v>25</v>
+      </c>
+      <c r="N30" s="4">
+        <v>26</v>
+      </c>
+      <c r="O30" s="4">
+        <v>27</v>
+      </c>
+      <c r="P30" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q30" s="4">
+        <v>1</v>
+      </c>
+      <c r="R30" s="4">
+        <v>2</v>
+      </c>
+      <c r="S30" s="4">
+        <v>2</v>
+      </c>
+      <c r="T30" s="4">
+        <v>2</v>
+      </c>
+      <c r="U30" s="4">
+        <v>2</v>
+      </c>
+      <c r="V30" s="4">
+        <v>2</v>
+      </c>
+      <c r="W30" s="4">
+        <v>2</v>
+      </c>
+      <c r="X30" s="4">
+        <v>2</v>
+      </c>
+      <c r="Y30" s="4">
+        <v>2</v>
+      </c>
+      <c r="Z30" s="4">
+        <v>2</v>
+      </c>
+      <c r="AA30" s="4">
+        <v>2</v>
+      </c>
+      <c r="AB30" s="3"/>
+      <c r="AC30" s="3"/>
+      <c r="AD30" s="2"/>
+      <c r="AE30" s="2"/>
+    </row>
+    <row r="31" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A31" s="1">
+        <f t="shared" si="31"/>
+        <v>5</v>
+      </c>
+      <c r="B31" s="2"/>
+      <c r="C31" s="2"/>
+      <c r="D31" s="3"/>
+      <c r="E31" s="3"/>
+      <c r="F31" s="4">
+        <v>18</v>
+      </c>
+      <c r="G31" s="4">
+        <v>19</v>
+      </c>
+      <c r="H31" s="4">
+        <v>20</v>
+      </c>
+      <c r="I31" s="4">
+        <v>21</v>
+      </c>
+      <c r="J31" s="4">
+        <v>22</v>
+      </c>
+      <c r="K31" s="4">
+        <v>23</v>
+      </c>
+      <c r="L31" s="4">
+        <v>24</v>
+      </c>
+      <c r="M31" s="4">
+        <v>25</v>
+      </c>
+      <c r="N31" s="4">
+        <v>26</v>
+      </c>
+      <c r="O31" s="4">
+        <v>27</v>
+      </c>
+      <c r="P31" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q31" s="4">
+        <v>1</v>
+      </c>
+      <c r="R31" s="4">
+        <v>2</v>
+      </c>
+      <c r="S31" s="4">
+        <v>3</v>
+      </c>
+      <c r="T31" s="4">
+        <v>3</v>
+      </c>
+      <c r="U31" s="4">
+        <v>3</v>
+      </c>
+      <c r="V31" s="4">
+        <v>3</v>
+      </c>
+      <c r="W31" s="4">
+        <v>3</v>
+      </c>
+      <c r="X31" s="4">
+        <v>3</v>
+      </c>
+      <c r="Y31" s="4">
+        <v>3</v>
+      </c>
+      <c r="Z31" s="4">
+        <v>3</v>
+      </c>
+      <c r="AA31" s="4">
+        <v>3</v>
+      </c>
+      <c r="AB31" s="3"/>
+      <c r="AC31" s="3"/>
+      <c r="AD31" s="2"/>
+      <c r="AE31" s="2"/>
+    </row>
+    <row r="32" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A32" s="1">
+        <f t="shared" si="31"/>
+        <v>6</v>
+      </c>
+      <c r="B32" s="2"/>
+      <c r="C32" s="2"/>
+      <c r="D32" s="3"/>
+      <c r="E32" s="3"/>
+      <c r="F32" s="4">
+        <v>18</v>
+      </c>
+      <c r="G32" s="4">
+        <v>19</v>
+      </c>
+      <c r="H32" s="4">
+        <v>20</v>
+      </c>
+      <c r="I32" s="4">
+        <v>21</v>
+      </c>
+      <c r="J32" s="4">
+        <v>22</v>
+      </c>
+      <c r="K32" s="4">
+        <v>23</v>
+      </c>
+      <c r="L32" s="4">
+        <v>24</v>
+      </c>
+      <c r="M32" s="4">
+        <v>25</v>
+      </c>
+      <c r="N32" s="4">
+        <v>26</v>
+      </c>
+      <c r="O32" s="4">
+        <v>27</v>
+      </c>
+      <c r="P32" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q32" s="4">
+        <v>1</v>
+      </c>
+      <c r="R32" s="4">
+        <v>2</v>
+      </c>
+      <c r="S32" s="4">
+        <v>3</v>
+      </c>
+      <c r="T32" s="4">
+        <v>4</v>
+      </c>
+      <c r="U32" s="4">
+        <v>4</v>
+      </c>
+      <c r="V32" s="4">
+        <v>4</v>
+      </c>
+      <c r="W32" s="4">
+        <v>4</v>
+      </c>
+      <c r="X32" s="4">
+        <v>4</v>
+      </c>
+      <c r="Y32" s="4">
+        <v>4</v>
+      </c>
+      <c r="Z32" s="4">
+        <v>4</v>
+      </c>
+      <c r="AA32" s="4">
+        <v>4</v>
+      </c>
+      <c r="AB32" s="3"/>
+      <c r="AC32" s="3"/>
+      <c r="AD32" s="2"/>
+      <c r="AE32" s="2"/>
+    </row>
+    <row r="33" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A33" s="1">
+        <f t="shared" si="31"/>
+        <v>7</v>
+      </c>
+      <c r="B33" s="2"/>
+      <c r="C33" s="2"/>
+      <c r="D33" s="3"/>
+      <c r="E33" s="3"/>
+      <c r="F33" s="4">
+        <v>18</v>
+      </c>
+      <c r="G33" s="4">
+        <v>19</v>
+      </c>
+      <c r="H33" s="4">
+        <v>20</v>
+      </c>
+      <c r="I33" s="4">
+        <v>21</v>
+      </c>
+      <c r="J33" s="4">
+        <v>22</v>
+      </c>
+      <c r="K33" s="4">
+        <v>23</v>
+      </c>
+      <c r="L33" s="4">
+        <v>24</v>
+      </c>
+      <c r="M33" s="3"/>
+      <c r="N33" s="2"/>
+      <c r="O33" s="2"/>
+      <c r="P33" s="2"/>
+      <c r="Q33" s="2"/>
+      <c r="R33" s="3"/>
+      <c r="S33" s="3"/>
+      <c r="T33" s="3"/>
+      <c r="U33" s="4">
+        <v>5</v>
+      </c>
+      <c r="V33" s="4">
+        <v>5</v>
+      </c>
+      <c r="W33" s="4">
+        <v>5</v>
+      </c>
+      <c r="X33" s="4">
+        <v>5</v>
+      </c>
+      <c r="Y33" s="4">
+        <v>5</v>
+      </c>
+      <c r="Z33" s="4">
+        <v>5</v>
+      </c>
+      <c r="AA33" s="4">
+        <v>4</v>
+      </c>
+      <c r="AB33" s="3"/>
+      <c r="AC33" s="3"/>
+      <c r="AD33" s="2"/>
+      <c r="AE33" s="2"/>
+    </row>
+    <row r="34" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A34" s="1">
+        <f t="shared" si="31"/>
+        <v>8</v>
+      </c>
+      <c r="B34" s="2"/>
+      <c r="C34" s="2"/>
+      <c r="D34" s="3"/>
+      <c r="E34" s="3"/>
+      <c r="F34" s="4">
+        <v>18</v>
+      </c>
+      <c r="G34" s="4">
+        <v>19</v>
+      </c>
+      <c r="H34" s="4">
+        <v>20</v>
+      </c>
+      <c r="I34" s="4">
+        <v>21</v>
+      </c>
+      <c r="J34" s="4">
+        <v>22</v>
+      </c>
+      <c r="K34" s="4">
+        <v>23</v>
+      </c>
+      <c r="L34" s="4">
+        <v>23</v>
+      </c>
+      <c r="M34" s="3"/>
+      <c r="N34" s="2"/>
+      <c r="O34" s="2"/>
+      <c r="P34" s="2"/>
+      <c r="Q34" s="2"/>
+      <c r="R34" s="3"/>
+      <c r="S34" s="3"/>
+      <c r="T34" s="3"/>
+      <c r="U34" s="4">
+        <v>6</v>
+      </c>
+      <c r="V34" s="4">
+        <v>6</v>
+      </c>
+      <c r="W34" s="4">
+        <v>6</v>
+      </c>
+      <c r="X34" s="4">
+        <v>6</v>
+      </c>
+      <c r="Y34" s="4">
+        <v>6</v>
+      </c>
+      <c r="Z34" s="4">
+        <v>5</v>
+      </c>
+      <c r="AA34" s="4">
+        <v>4</v>
+      </c>
+      <c r="AB34" s="3"/>
+      <c r="AC34" s="3"/>
+      <c r="AD34" s="2"/>
+      <c r="AE34" s="2"/>
+    </row>
+    <row r="35" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A35" s="1">
+        <f t="shared" si="31"/>
+        <v>9</v>
+      </c>
+      <c r="B35" s="2"/>
+      <c r="C35" s="2"/>
+      <c r="D35" s="3"/>
+      <c r="E35" s="3"/>
+      <c r="F35" s="4">
+        <v>18</v>
+      </c>
+      <c r="G35" s="4">
+        <v>19</v>
+      </c>
+      <c r="H35" s="4">
+        <v>20</v>
+      </c>
+      <c r="I35" s="4">
+        <v>21</v>
+      </c>
+      <c r="J35" s="4">
+        <v>22</v>
+      </c>
+      <c r="K35" s="4">
+        <v>22</v>
+      </c>
+      <c r="L35" s="4">
+        <v>22</v>
+      </c>
+      <c r="M35" s="3"/>
+      <c r="N35" s="3"/>
+      <c r="O35" s="2"/>
+      <c r="P35" s="2"/>
+      <c r="Q35" s="2"/>
+      <c r="R35" s="2"/>
+      <c r="S35" s="3"/>
+      <c r="T35" s="3"/>
+      <c r="U35" s="4">
+        <v>7</v>
+      </c>
+      <c r="V35" s="4">
+        <v>7</v>
+      </c>
+      <c r="W35" s="4">
+        <v>7</v>
+      </c>
+      <c r="X35" s="4">
+        <v>7</v>
+      </c>
+      <c r="Y35" s="4">
+        <v>6</v>
+      </c>
+      <c r="Z35" s="4">
+        <v>5</v>
+      </c>
+      <c r="AA35" s="4">
+        <v>4</v>
+      </c>
+      <c r="AB35" s="3"/>
+      <c r="AC35" s="3"/>
+      <c r="AD35" s="2"/>
+      <c r="AE35" s="2"/>
+    </row>
+    <row r="36" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A36" s="1">
+        <f t="shared" si="31"/>
+        <v>10</v>
+      </c>
+      <c r="B36" s="2"/>
+      <c r="C36" s="2"/>
+      <c r="D36" s="3"/>
+      <c r="E36" s="3"/>
+      <c r="F36" s="4">
+        <v>18</v>
+      </c>
+      <c r="G36" s="4">
+        <v>19</v>
+      </c>
+      <c r="H36" s="4">
+        <v>20</v>
+      </c>
+      <c r="I36" s="4">
+        <v>21</v>
+      </c>
+      <c r="J36" s="4">
+        <v>21</v>
+      </c>
+      <c r="K36" s="4">
+        <v>21</v>
+      </c>
+      <c r="L36" s="4">
+        <v>21</v>
+      </c>
+      <c r="M36" s="3"/>
+      <c r="N36" s="3"/>
+      <c r="O36" s="2"/>
+      <c r="P36" s="2"/>
+      <c r="Q36" s="2"/>
+      <c r="R36" s="2"/>
+      <c r="S36" s="3"/>
+      <c r="T36" s="3"/>
+      <c r="U36" s="4">
+        <v>8</v>
+      </c>
+      <c r="V36" s="4">
+        <v>8</v>
+      </c>
+      <c r="W36" s="4">
+        <v>8</v>
+      </c>
+      <c r="X36" s="4">
+        <v>7</v>
+      </c>
+      <c r="Y36" s="4">
+        <v>6</v>
+      </c>
+      <c r="Z36" s="4">
+        <v>5</v>
+      </c>
+      <c r="AA36" s="4">
+        <v>4</v>
+      </c>
+      <c r="AB36" s="3"/>
+      <c r="AC36" s="3"/>
+      <c r="AD36" s="2"/>
+      <c r="AE36" s="2"/>
+    </row>
+    <row r="37" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A37" s="1">
+        <f t="shared" si="31"/>
+        <v>11</v>
+      </c>
+      <c r="B37" s="2"/>
+      <c r="C37" s="2"/>
+      <c r="D37" s="3"/>
+      <c r="E37" s="3"/>
+      <c r="F37" s="4">
+        <v>18</v>
+      </c>
+      <c r="G37" s="4">
+        <v>19</v>
+      </c>
+      <c r="H37" s="4">
+        <v>20</v>
+      </c>
+      <c r="I37" s="4">
+        <v>20</v>
+      </c>
+      <c r="J37" s="4">
+        <v>20</v>
+      </c>
+      <c r="K37" s="4">
+        <v>20</v>
+      </c>
+      <c r="L37" s="4">
+        <v>20</v>
+      </c>
+      <c r="M37" s="3"/>
+      <c r="N37" s="3"/>
+      <c r="O37" s="3"/>
+      <c r="P37" s="3"/>
+      <c r="Q37" s="3"/>
+      <c r="R37" s="3"/>
+      <c r="S37" s="3"/>
+      <c r="T37" s="3"/>
+      <c r="U37" s="4">
+        <v>9</v>
+      </c>
+      <c r="V37" s="4">
+        <v>9</v>
+      </c>
+      <c r="W37" s="4">
+        <v>8</v>
+      </c>
+      <c r="X37" s="4">
+        <v>7</v>
+      </c>
+      <c r="Y37" s="4">
+        <v>6</v>
+      </c>
+      <c r="Z37" s="4">
+        <v>5</v>
+      </c>
+      <c r="AA37" s="4">
+        <v>4</v>
+      </c>
+      <c r="AB37" s="3"/>
+      <c r="AC37" s="3"/>
+      <c r="AD37" s="2"/>
+      <c r="AE37" s="2"/>
+    </row>
+    <row r="38" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A38" s="1">
+        <f t="shared" si="31"/>
+        <v>12</v>
+      </c>
+      <c r="B38" s="2"/>
+      <c r="C38" s="2"/>
+      <c r="D38" s="3"/>
+      <c r="E38" s="3"/>
+      <c r="F38" s="4">
+        <v>18</v>
+      </c>
+      <c r="G38" s="4">
+        <v>19</v>
+      </c>
+      <c r="H38" s="4">
+        <v>19</v>
+      </c>
+      <c r="I38" s="4">
+        <v>19</v>
+      </c>
+      <c r="J38" s="4">
+        <v>19</v>
+      </c>
+      <c r="K38" s="4">
+        <v>19</v>
+      </c>
+      <c r="L38" s="4">
+        <v>19</v>
+      </c>
+      <c r="M38" s="3"/>
+      <c r="N38" s="3"/>
+      <c r="O38" s="3"/>
+      <c r="P38" s="3"/>
+      <c r="Q38" s="3"/>
+      <c r="R38" s="3"/>
+      <c r="S38" s="3"/>
+      <c r="T38" s="3"/>
+      <c r="U38" s="4">
+        <v>10</v>
+      </c>
+      <c r="V38" s="4">
+        <v>9</v>
+      </c>
+      <c r="W38" s="4">
+        <v>8</v>
+      </c>
+      <c r="X38" s="4">
+        <v>7</v>
+      </c>
+      <c r="Y38" s="4">
+        <v>6</v>
+      </c>
+      <c r="Z38" s="4">
+        <v>5</v>
+      </c>
+      <c r="AA38" s="4">
+        <v>4</v>
+      </c>
+      <c r="AB38" s="3"/>
+      <c r="AC38" s="3"/>
+      <c r="AD38" s="2"/>
+      <c r="AE38" s="2"/>
+    </row>
+    <row r="39" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A39" s="1">
+        <f t="shared" si="31"/>
+        <v>13</v>
+      </c>
+      <c r="B39" s="2"/>
+      <c r="C39" s="2"/>
+      <c r="D39" s="3"/>
+      <c r="E39" s="3"/>
+      <c r="F39" s="4">
+        <v>18</v>
+      </c>
+      <c r="G39" s="4">
+        <v>18</v>
+      </c>
+      <c r="H39" s="4">
+        <v>18</v>
+      </c>
+      <c r="I39" s="4">
+        <v>18</v>
+      </c>
+      <c r="J39" s="4">
+        <v>18</v>
+      </c>
+      <c r="K39" s="4">
+        <v>18</v>
+      </c>
+      <c r="L39" s="4">
+        <v>18</v>
+      </c>
+      <c r="M39" s="4">
+        <v>18</v>
+      </c>
+      <c r="N39" s="4">
+        <v>17</v>
+      </c>
+      <c r="O39" s="4">
+        <v>16</v>
+      </c>
+      <c r="P39" s="4">
+        <v>15</v>
+      </c>
+      <c r="Q39" s="4">
+        <v>14</v>
+      </c>
+      <c r="R39" s="4">
+        <v>13</v>
+      </c>
+      <c r="S39" s="4">
+        <v>12</v>
+      </c>
+      <c r="T39" s="4">
+        <v>11</v>
+      </c>
+      <c r="U39" s="4">
+        <v>10</v>
+      </c>
+      <c r="V39" s="4">
+        <v>9</v>
+      </c>
+      <c r="W39" s="4">
+        <v>8</v>
+      </c>
+      <c r="X39" s="4">
+        <v>7</v>
+      </c>
+      <c r="Y39" s="4">
+        <v>6</v>
+      </c>
+      <c r="Z39" s="4">
+        <v>5</v>
+      </c>
+      <c r="AA39" s="4">
+        <v>4</v>
+      </c>
+      <c r="AB39" s="3"/>
+      <c r="AC39" s="3"/>
+      <c r="AD39" s="2"/>
+      <c r="AE39" s="2"/>
+    </row>
+    <row r="40" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A40" s="1">
+        <f t="shared" si="31"/>
+        <v>14</v>
+      </c>
+      <c r="B40" s="2"/>
+      <c r="C40" s="2"/>
+      <c r="D40" s="3"/>
+      <c r="E40" s="3"/>
+      <c r="F40" s="4">
+        <v>17</v>
+      </c>
+      <c r="G40" s="4">
+        <v>17</v>
+      </c>
+      <c r="H40" s="4">
+        <v>17</v>
+      </c>
+      <c r="I40" s="4">
+        <v>17</v>
+      </c>
+      <c r="J40" s="4">
+        <v>17</v>
+      </c>
+      <c r="K40" s="4">
+        <v>17</v>
+      </c>
+      <c r="L40" s="4">
+        <v>17</v>
+      </c>
+      <c r="M40" s="4">
+        <v>17</v>
+      </c>
+      <c r="N40" s="4">
+        <v>17</v>
+      </c>
+      <c r="O40" s="4">
+        <v>16</v>
+      </c>
+      <c r="P40" s="4">
+        <v>15</v>
+      </c>
+      <c r="Q40" s="4">
+        <v>14</v>
+      </c>
+      <c r="R40" s="4">
+        <v>13</v>
+      </c>
+      <c r="S40" s="4">
+        <v>12</v>
+      </c>
+      <c r="T40" s="4">
+        <v>11</v>
+      </c>
+      <c r="U40" s="4">
+        <v>10</v>
+      </c>
+      <c r="V40" s="4">
+        <v>9</v>
+      </c>
+      <c r="W40" s="4">
+        <v>8</v>
+      </c>
+      <c r="X40" s="4">
+        <v>7</v>
+      </c>
+      <c r="Y40" s="4">
+        <v>6</v>
+      </c>
+      <c r="Z40" s="4">
+        <v>5</v>
+      </c>
+      <c r="AA40" s="4">
+        <v>4</v>
+      </c>
+      <c r="AB40" s="3"/>
+      <c r="AC40" s="3"/>
+      <c r="AD40" s="2"/>
+      <c r="AE40" s="2"/>
+    </row>
+    <row r="41" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A41" s="1">
+        <f t="shared" si="31"/>
+        <v>15</v>
+      </c>
+      <c r="B41" s="2"/>
+      <c r="C41" s="2"/>
+      <c r="D41" s="3"/>
+      <c r="E41" s="3"/>
+      <c r="F41" s="4">
+        <v>16</v>
+      </c>
+      <c r="G41" s="4">
+        <v>16</v>
+      </c>
+      <c r="H41" s="4">
+        <v>16</v>
+      </c>
+      <c r="I41" s="4">
+        <v>16</v>
+      </c>
+      <c r="J41" s="4">
+        <v>16</v>
+      </c>
+      <c r="K41" s="4">
+        <v>16</v>
+      </c>
+      <c r="L41" s="4">
+        <v>16</v>
+      </c>
+      <c r="M41" s="4">
+        <v>16</v>
+      </c>
+      <c r="N41" s="4">
+        <v>16</v>
+      </c>
+      <c r="O41" s="4">
+        <v>16</v>
+      </c>
+      <c r="P41" s="4">
+        <v>15</v>
+      </c>
+      <c r="Q41" s="4">
+        <v>14</v>
+      </c>
+      <c r="R41" s="4">
+        <v>13</v>
+      </c>
+      <c r="S41" s="4">
+        <v>12</v>
+      </c>
+      <c r="T41" s="4">
+        <v>11</v>
+      </c>
+      <c r="U41" s="4">
+        <v>10</v>
+      </c>
+      <c r="V41" s="4">
+        <v>9</v>
+      </c>
+      <c r="W41" s="4">
+        <v>8</v>
+      </c>
+      <c r="X41" s="4">
+        <v>7</v>
+      </c>
+      <c r="Y41" s="4">
+        <v>6</v>
+      </c>
+      <c r="Z41" s="4">
+        <v>5</v>
+      </c>
+      <c r="AA41" s="4">
+        <v>4</v>
+      </c>
+      <c r="AB41" s="3"/>
+      <c r="AC41" s="3"/>
+      <c r="AD41" s="2"/>
+      <c r="AE41" s="2"/>
+    </row>
+    <row r="42" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A42" s="1">
+        <f t="shared" si="31"/>
+        <v>16</v>
+      </c>
+      <c r="B42" s="2"/>
+      <c r="C42" s="2"/>
+      <c r="D42" s="3"/>
+      <c r="E42" s="3"/>
+      <c r="F42" s="3"/>
+      <c r="G42" s="3"/>
+      <c r="H42" s="3"/>
+      <c r="I42" s="3"/>
+      <c r="J42" s="3"/>
+      <c r="K42" s="3"/>
+      <c r="L42" s="3"/>
+      <c r="M42" s="3"/>
+      <c r="N42" s="3"/>
+      <c r="O42" s="3"/>
+      <c r="P42" s="3"/>
+      <c r="Q42" s="3"/>
+      <c r="R42" s="3"/>
+      <c r="S42" s="3"/>
+      <c r="T42" s="3"/>
+      <c r="U42" s="3"/>
+      <c r="V42" s="3"/>
+      <c r="W42" s="3"/>
+      <c r="X42" s="3"/>
+      <c r="Y42" s="3"/>
+      <c r="Z42" s="3"/>
+      <c r="AA42" s="3"/>
+      <c r="AB42" s="3"/>
+      <c r="AC42" s="3"/>
+      <c r="AD42" s="2"/>
+      <c r="AE42" s="2"/>
+    </row>
+    <row r="43" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A43" s="1">
+        <f t="shared" si="31"/>
+        <v>17</v>
+      </c>
+      <c r="B43" s="2"/>
+      <c r="C43" s="2"/>
+      <c r="D43" s="3"/>
+      <c r="E43" s="3"/>
+      <c r="F43" s="3"/>
+      <c r="G43" s="3"/>
+      <c r="H43" s="3"/>
+      <c r="I43" s="3"/>
+      <c r="J43" s="3"/>
+      <c r="K43" s="3"/>
+      <c r="L43" s="3"/>
+      <c r="M43" s="3"/>
+      <c r="N43" s="3"/>
+      <c r="O43" s="3"/>
+      <c r="P43" s="3"/>
+      <c r="Q43" s="3"/>
+      <c r="R43" s="3"/>
+      <c r="S43" s="3"/>
+      <c r="T43" s="3"/>
+      <c r="U43" s="3"/>
+      <c r="V43" s="3"/>
+      <c r="W43" s="3"/>
+      <c r="X43" s="3"/>
+      <c r="Y43" s="3"/>
+      <c r="Z43" s="3"/>
+      <c r="AA43" s="3"/>
+      <c r="AB43" s="3"/>
+      <c r="AC43" s="3"/>
+      <c r="AD43" s="2"/>
+      <c r="AE43" s="2"/>
+    </row>
+    <row r="44" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A44" s="1">
+        <f t="shared" si="31"/>
+        <v>18</v>
+      </c>
+      <c r="B44" s="2"/>
+      <c r="C44" s="2"/>
+      <c r="D44" s="2"/>
+      <c r="E44" s="2"/>
+      <c r="F44" s="2"/>
+      <c r="G44" s="2"/>
+      <c r="H44" s="2"/>
+      <c r="I44" s="2"/>
+      <c r="J44" s="2"/>
+      <c r="K44" s="2"/>
+      <c r="L44" s="2"/>
+      <c r="M44" s="2"/>
+      <c r="N44" s="2"/>
+      <c r="O44" s="2"/>
+      <c r="P44" s="2"/>
+      <c r="Q44" s="2"/>
+      <c r="R44" s="2"/>
+      <c r="S44" s="2"/>
+      <c r="T44" s="2"/>
+      <c r="U44" s="2"/>
+      <c r="V44" s="2"/>
+      <c r="W44" s="2"/>
+      <c r="X44" s="2"/>
+      <c r="Y44" s="2"/>
+      <c r="Z44" s="2"/>
+      <c r="AA44" s="2"/>
+      <c r="AB44" s="2"/>
+      <c r="AC44" s="2"/>
+      <c r="AD44" s="2"/>
+      <c r="AE44" s="2"/>
+    </row>
+    <row r="45" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A45" s="1">
+        <f t="shared" si="31"/>
+        <v>19</v>
+      </c>
+      <c r="B45" s="2"/>
+      <c r="C45" s="2"/>
+      <c r="D45" s="2"/>
+      <c r="E45" s="2"/>
+      <c r="F45" s="2"/>
+      <c r="G45" s="2"/>
+      <c r="H45" s="2"/>
+      <c r="I45" s="2"/>
+      <c r="J45" s="2"/>
+      <c r="K45" s="2"/>
+      <c r="L45" s="2"/>
+      <c r="M45" s="2"/>
+      <c r="N45" s="2"/>
+      <c r="O45" s="2"/>
+      <c r="P45" s="2"/>
+      <c r="Q45" s="2"/>
+      <c r="R45" s="2"/>
+      <c r="S45" s="2"/>
+      <c r="T45" s="2"/>
+      <c r="U45" s="2"/>
+      <c r="V45" s="2"/>
+      <c r="W45" s="2"/>
+      <c r="X45" s="2"/>
+      <c r="Y45" s="2"/>
+      <c r="Z45" s="2"/>
+      <c r="AA45" s="2"/>
+      <c r="AB45" s="2"/>
+      <c r="AC45" s="2"/>
+      <c r="AD45" s="2"/>
+      <c r="AE45" s="2"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>